<commit_message>
Casi completo solo falta repetir las paginas de familia y cerrar ciclos
</commit_message>
<xml_diff>
--- a/Libro1.xlsx
+++ b/Libro1.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\mobileQuest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{D2621C20-142E-46C7-A863-5BEC64CB8076}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{EC9B4606-6F63-46F6-B801-A67042F698E2}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" xr2:uid="{0D3B767B-82B4-4727-A6C9-A3D8FEE55BBD}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" activeTab="1" xr2:uid="{0D3B767B-82B4-4727-A6C9-A3D8FEE55BBD}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="81">
   <si>
     <t>'".</t>
   </si>
@@ -150,48 +151,6 @@
     <t>$p51</t>
   </si>
   <si>
-    <t>p86</t>
-  </si>
-  <si>
-    <t>p87</t>
-  </si>
-  <si>
-    <t>p88</t>
-  </si>
-  <si>
-    <t>p89</t>
-  </si>
-  <si>
-    <t>p90</t>
-  </si>
-  <si>
-    <t>p91</t>
-  </si>
-  <si>
-    <t>p92</t>
-  </si>
-  <si>
-    <t>p93</t>
-  </si>
-  <si>
-    <t>p94</t>
-  </si>
-  <si>
-    <t>p95</t>
-  </si>
-  <si>
-    <t>p96</t>
-  </si>
-  <si>
-    <t>p97</t>
-  </si>
-  <si>
-    <t>p98</t>
-  </si>
-  <si>
-    <t>p99</t>
-  </si>
-  <si>
     <t>p100</t>
   </si>
   <si>
@@ -259,6 +218,57 @@
   </si>
   <si>
     <t>p122</t>
+  </si>
+  <si>
+    <t>p1_52</t>
+  </si>
+  <si>
+    <t>p1_53</t>
+  </si>
+  <si>
+    <t>p1_54</t>
+  </si>
+  <si>
+    <t>p1_55</t>
+  </si>
+  <si>
+    <t>p1_56</t>
+  </si>
+  <si>
+    <t>p1_57</t>
+  </si>
+  <si>
+    <t>p1_58</t>
+  </si>
+  <si>
+    <t>p1_59</t>
+  </si>
+  <si>
+    <t>p1_60</t>
+  </si>
+  <si>
+    <t>p1_61</t>
+  </si>
+  <si>
+    <t>p1_62</t>
+  </si>
+  <si>
+    <t>p1_63</t>
+  </si>
+  <si>
+    <t>p1_64</t>
+  </si>
+  <si>
+    <t>p1_65</t>
+  </si>
+  <si>
+    <t>$</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> = $_POST['</t>
+  </si>
+  <si>
+    <t>'];</t>
   </si>
 </sst>
 </file>
@@ -613,8 +623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4182BBE6-465C-4753-81EF-2A668EF48C3E}">
   <dimension ref="A1:R37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E10" workbookViewId="0">
-      <selection activeCell="R21" sqref="R21:R36"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1:O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -647,10 +657,10 @@
       </c>
       <c r="K1" t="str">
         <f>CONCATENATE(G1,L1,I1,L1,J1)</f>
-        <v>echo $p86."=p86&lt;br&gt;";</v>
+        <v>echo $p1_52."=p1_52&lt;br&gt;";</v>
       </c>
       <c r="L1" t="s">
-        <v>41</v>
+        <v>64</v>
       </c>
       <c r="M1" t="s">
         <v>26</v>
@@ -659,14 +669,14 @@
         <v>27</v>
       </c>
       <c r="O1" t="s">
-        <v>41</v>
+        <v>64</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>28</v>
       </c>
       <c r="R1" t="str">
         <f>CONCATENATE(L1,M1,N1,O1,P1)</f>
-        <v>p86='$p86',</v>
+        <v>p1_52='$p1_52',</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -694,10 +704,10 @@
       </c>
       <c r="K2" t="str">
         <f t="shared" ref="K2:K33" si="1">CONCATENATE(G2,L2,I2,L2,J2)</f>
-        <v>echo $p87."=p87&lt;br&gt;";</v>
+        <v>echo $p1_53."=p1_53&lt;br&gt;";</v>
       </c>
       <c r="L2" t="s">
-        <v>42</v>
+        <v>65</v>
       </c>
       <c r="M2" t="s">
         <v>26</v>
@@ -706,14 +716,14 @@
         <v>27</v>
       </c>
       <c r="O2" t="s">
-        <v>42</v>
+        <v>65</v>
       </c>
       <c r="P2" s="1" t="s">
         <v>28</v>
       </c>
       <c r="R2" t="str">
         <f t="shared" ref="R2:R33" si="2">CONCATENATE(L2,M2,N2,O2,P2)</f>
-        <v>p87='$p87',</v>
+        <v>p1_53='$p1_53',</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -741,10 +751,10 @@
       </c>
       <c r="K3" t="str">
         <f t="shared" si="1"/>
-        <v>echo $p88."=p88&lt;br&gt;";</v>
+        <v>echo $p1_54."=p1_54&lt;br&gt;";</v>
       </c>
       <c r="L3" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="M3" t="s">
         <v>26</v>
@@ -753,14 +763,14 @@
         <v>27</v>
       </c>
       <c r="O3" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="P3" s="1" t="s">
         <v>28</v>
       </c>
       <c r="R3" t="str">
         <f t="shared" si="2"/>
-        <v>p88='$p88',</v>
+        <v>p1_54='$p1_54',</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -788,10 +798,10 @@
       </c>
       <c r="K4" t="str">
         <f t="shared" si="1"/>
-        <v>echo $p89."=p89&lt;br&gt;";</v>
+        <v>echo $p1_55."=p1_55&lt;br&gt;";</v>
       </c>
       <c r="L4" t="s">
-        <v>44</v>
+        <v>67</v>
       </c>
       <c r="M4" t="s">
         <v>26</v>
@@ -800,14 +810,14 @@
         <v>27</v>
       </c>
       <c r="O4" t="s">
-        <v>44</v>
+        <v>67</v>
       </c>
       <c r="P4" s="1" t="s">
         <v>28</v>
       </c>
       <c r="R4" t="str">
         <f t="shared" si="2"/>
-        <v>p89='$p89',</v>
+        <v>p1_55='$p1_55',</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
@@ -835,10 +845,10 @@
       </c>
       <c r="K5" t="str">
         <f t="shared" si="1"/>
-        <v>echo $p90."=p90&lt;br&gt;";</v>
+        <v>echo $p1_56."=p1_56&lt;br&gt;";</v>
       </c>
       <c r="L5" t="s">
-        <v>45</v>
+        <v>68</v>
       </c>
       <c r="M5" t="s">
         <v>26</v>
@@ -847,14 +857,14 @@
         <v>27</v>
       </c>
       <c r="O5" t="s">
-        <v>45</v>
+        <v>68</v>
       </c>
       <c r="P5" s="1" t="s">
         <v>28</v>
       </c>
       <c r="R5" t="str">
         <f t="shared" si="2"/>
-        <v>p90='$p90',</v>
+        <v>p1_56='$p1_56',</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -882,10 +892,10 @@
       </c>
       <c r="K6" t="str">
         <f t="shared" si="1"/>
-        <v>echo $p91."=p91&lt;br&gt;";</v>
+        <v>echo $p1_57."=p1_57&lt;br&gt;";</v>
       </c>
       <c r="L6" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="M6" t="s">
         <v>26</v>
@@ -894,14 +904,14 @@
         <v>27</v>
       </c>
       <c r="O6" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="P6" s="1" t="s">
         <v>28</v>
       </c>
       <c r="R6" t="str">
         <f t="shared" si="2"/>
-        <v>p91='$p91',</v>
+        <v>p1_57='$p1_57',</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -929,10 +939,10 @@
       </c>
       <c r="K7" t="str">
         <f t="shared" si="1"/>
-        <v>echo $p92."=p92&lt;br&gt;";</v>
+        <v>echo $p1_58."=p1_58&lt;br&gt;";</v>
       </c>
       <c r="L7" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="M7" t="s">
         <v>26</v>
@@ -941,14 +951,14 @@
         <v>27</v>
       </c>
       <c r="O7" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="P7" s="1" t="s">
         <v>28</v>
       </c>
       <c r="R7" t="str">
         <f t="shared" si="2"/>
-        <v>p92='$p92',</v>
+        <v>p1_58='$p1_58',</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
@@ -976,10 +986,10 @@
       </c>
       <c r="K8" t="str">
         <f t="shared" si="1"/>
-        <v>echo $p93."=p93&lt;br&gt;";</v>
+        <v>echo $p1_59."=p1_59&lt;br&gt;";</v>
       </c>
       <c r="L8" t="s">
-        <v>48</v>
+        <v>71</v>
       </c>
       <c r="M8" t="s">
         <v>26</v>
@@ -988,14 +998,14 @@
         <v>27</v>
       </c>
       <c r="O8" t="s">
-        <v>48</v>
+        <v>71</v>
       </c>
       <c r="P8" s="1" t="s">
         <v>28</v>
       </c>
       <c r="R8" t="str">
         <f t="shared" si="2"/>
-        <v>p93='$p93',</v>
+        <v>p1_59='$p1_59',</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -1023,10 +1033,10 @@
       </c>
       <c r="K9" t="str">
         <f t="shared" si="1"/>
-        <v>echo $p94."=p94&lt;br&gt;";</v>
+        <v>echo $p1_60."=p1_60&lt;br&gt;";</v>
       </c>
       <c r="L9" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
       <c r="M9" t="s">
         <v>26</v>
@@ -1035,14 +1045,14 @@
         <v>27</v>
       </c>
       <c r="O9" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
       <c r="P9" s="1" t="s">
         <v>28</v>
       </c>
       <c r="R9" t="str">
         <f t="shared" si="2"/>
-        <v>p94='$p94',</v>
+        <v>p1_60='$p1_60',</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
@@ -1070,10 +1080,10 @@
       </c>
       <c r="K10" t="str">
         <f t="shared" si="1"/>
-        <v>echo $p95."=p95&lt;br&gt;";</v>
+        <v>echo $p1_61."=p1_61&lt;br&gt;";</v>
       </c>
       <c r="L10" t="s">
-        <v>50</v>
+        <v>73</v>
       </c>
       <c r="M10" t="s">
         <v>26</v>
@@ -1082,14 +1092,14 @@
         <v>27</v>
       </c>
       <c r="O10" t="s">
-        <v>50</v>
+        <v>73</v>
       </c>
       <c r="P10" s="1" t="s">
         <v>28</v>
       </c>
       <c r="R10" t="str">
         <f t="shared" si="2"/>
-        <v>p95='$p95',</v>
+        <v>p1_61='$p1_61',</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
@@ -1117,10 +1127,10 @@
       </c>
       <c r="K11" t="str">
         <f t="shared" si="1"/>
-        <v>echo $p96."=p96&lt;br&gt;";</v>
+        <v>echo $p1_62."=p1_62&lt;br&gt;";</v>
       </c>
       <c r="L11" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="M11" t="s">
         <v>26</v>
@@ -1129,14 +1139,14 @@
         <v>27</v>
       </c>
       <c r="O11" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="P11" s="1" t="s">
         <v>28</v>
       </c>
       <c r="R11" t="str">
         <f t="shared" si="2"/>
-        <v>p96='$p96',</v>
+        <v>p1_62='$p1_62',</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
@@ -1164,10 +1174,10 @@
       </c>
       <c r="K12" t="str">
         <f t="shared" si="1"/>
-        <v>echo $p97."=p97&lt;br&gt;";</v>
+        <v>echo $p1_63."=p1_63&lt;br&gt;";</v>
       </c>
       <c r="L12" t="s">
-        <v>52</v>
+        <v>75</v>
       </c>
       <c r="M12" t="s">
         <v>26</v>
@@ -1176,14 +1186,14 @@
         <v>27</v>
       </c>
       <c r="O12" t="s">
-        <v>52</v>
+        <v>75</v>
       </c>
       <c r="P12" s="1" t="s">
         <v>28</v>
       </c>
       <c r="R12" t="str">
         <f t="shared" si="2"/>
-        <v>p97='$p97',</v>
+        <v>p1_63='$p1_63',</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
@@ -1211,10 +1221,10 @@
       </c>
       <c r="K13" t="str">
         <f t="shared" si="1"/>
-        <v>echo $p98."=p98&lt;br&gt;";</v>
+        <v>echo $p1_64."=p1_64&lt;br&gt;";</v>
       </c>
       <c r="L13" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="M13" t="s">
         <v>26</v>
@@ -1223,14 +1233,14 @@
         <v>27</v>
       </c>
       <c r="O13" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="P13" s="1" t="s">
         <v>28</v>
       </c>
       <c r="R13" t="str">
         <f t="shared" si="2"/>
-        <v>p98='$p98',</v>
+        <v>p1_64='$p1_64',</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
@@ -1258,10 +1268,10 @@
       </c>
       <c r="K14" t="str">
         <f t="shared" si="1"/>
-        <v>echo $p99."=p99&lt;br&gt;";</v>
+        <v>echo $p1_65."=p1_65&lt;br&gt;";</v>
       </c>
       <c r="L14" t="s">
-        <v>54</v>
+        <v>77</v>
       </c>
       <c r="M14" t="s">
         <v>26</v>
@@ -1270,14 +1280,14 @@
         <v>27</v>
       </c>
       <c r="O14" t="s">
-        <v>54</v>
+        <v>77</v>
       </c>
       <c r="P14" s="1" t="s">
         <v>28</v>
       </c>
       <c r="R14" t="str">
         <f t="shared" si="2"/>
-        <v>p99='$p99',</v>
+        <v>p1_65='$p1_65',</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
@@ -1308,7 +1318,7 @@
         <v>echo $p100."=p100&lt;br&gt;";</v>
       </c>
       <c r="L15" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="M15" t="s">
         <v>26</v>
@@ -1317,7 +1327,7 @@
         <v>27</v>
       </c>
       <c r="O15" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="P15" s="1" t="s">
         <v>28</v>
@@ -1355,7 +1365,7 @@
         <v>echo $p101."=p101&lt;br&gt;";</v>
       </c>
       <c r="L16" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="M16" t="s">
         <v>26</v>
@@ -1364,7 +1374,7 @@
         <v>27</v>
       </c>
       <c r="O16" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="P16" s="1" t="s">
         <v>28</v>
@@ -1402,7 +1412,7 @@
         <v>echo $p102."=p102&lt;br&gt;";</v>
       </c>
       <c r="L17" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="M17" t="s">
         <v>26</v>
@@ -1411,7 +1421,7 @@
         <v>27</v>
       </c>
       <c r="O17" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="P17" s="1" t="s">
         <v>28</v>
@@ -1449,7 +1459,7 @@
         <v>echo $p103."=p103&lt;br&gt;";</v>
       </c>
       <c r="L18" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="M18" t="s">
         <v>26</v>
@@ -1458,7 +1468,7 @@
         <v>27</v>
       </c>
       <c r="O18" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="P18" s="1" t="s">
         <v>28</v>
@@ -1496,7 +1506,7 @@
         <v>echo $p104."=p104&lt;br&gt;";</v>
       </c>
       <c r="L19" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="M19" t="s">
         <v>26</v>
@@ -1505,7 +1515,7 @@
         <v>27</v>
       </c>
       <c r="O19" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="P19" s="1" t="s">
         <v>28</v>
@@ -1543,7 +1553,7 @@
         <v>echo $p105."=p105&lt;br&gt;";</v>
       </c>
       <c r="L20" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="M20" t="s">
         <v>26</v>
@@ -1552,7 +1562,7 @@
         <v>27</v>
       </c>
       <c r="O20" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="P20" s="1" t="s">
         <v>28</v>
@@ -1590,7 +1600,7 @@
         <v>echo $p106."=p106&lt;br&gt;";</v>
       </c>
       <c r="L21" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="M21" t="s">
         <v>26</v>
@@ -1599,7 +1609,7 @@
         <v>27</v>
       </c>
       <c r="O21" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="P21" s="1" t="s">
         <v>28</v>
@@ -1637,7 +1647,7 @@
         <v>echo $p107."=p107&lt;br&gt;";</v>
       </c>
       <c r="L22" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="M22" t="s">
         <v>26</v>
@@ -1646,7 +1656,7 @@
         <v>27</v>
       </c>
       <c r="O22" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="P22" s="1" t="s">
         <v>28</v>
@@ -1684,7 +1694,7 @@
         <v>echo $p108."=p108&lt;br&gt;";</v>
       </c>
       <c r="L23" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="M23" t="s">
         <v>26</v>
@@ -1693,7 +1703,7 @@
         <v>27</v>
       </c>
       <c r="O23" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="P23" s="1" t="s">
         <v>28</v>
@@ -1731,7 +1741,7 @@
         <v>echo $p109."=p109&lt;br&gt;";</v>
       </c>
       <c r="L24" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="M24" t="s">
         <v>26</v>
@@ -1740,7 +1750,7 @@
         <v>27</v>
       </c>
       <c r="O24" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="P24" s="1" t="s">
         <v>28</v>
@@ -1778,7 +1788,7 @@
         <v>echo $p110."=p110&lt;br&gt;";</v>
       </c>
       <c r="L25" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="M25" t="s">
         <v>26</v>
@@ -1787,7 +1797,7 @@
         <v>27</v>
       </c>
       <c r="O25" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="P25" s="1" t="s">
         <v>28</v>
@@ -1825,7 +1835,7 @@
         <v>echo $p111."=p111&lt;br&gt;";</v>
       </c>
       <c r="L26" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="M26" t="s">
         <v>26</v>
@@ -1834,7 +1844,7 @@
         <v>27</v>
       </c>
       <c r="O26" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="P26" s="1" t="s">
         <v>28</v>
@@ -1872,7 +1882,7 @@
         <v>echo $p112."=p112&lt;br&gt;";</v>
       </c>
       <c r="L27" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="M27" t="s">
         <v>26</v>
@@ -1881,7 +1891,7 @@
         <v>27</v>
       </c>
       <c r="O27" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="P27" s="1" t="s">
         <v>28</v>
@@ -1919,7 +1929,7 @@
         <v>echo $p113."=p113&lt;br&gt;";</v>
       </c>
       <c r="L28" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="M28" t="s">
         <v>26</v>
@@ -1928,7 +1938,7 @@
         <v>27</v>
       </c>
       <c r="O28" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="P28" s="1" t="s">
         <v>28</v>
@@ -1966,7 +1976,7 @@
         <v>echo $p114."=p114&lt;br&gt;";</v>
       </c>
       <c r="L29" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="M29" t="s">
         <v>26</v>
@@ -1975,7 +1985,7 @@
         <v>27</v>
       </c>
       <c r="O29" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="P29" s="1" t="s">
         <v>28</v>
@@ -2013,7 +2023,7 @@
         <v>echo $p115."=p115&lt;br&gt;";</v>
       </c>
       <c r="L30" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="M30" t="s">
         <v>26</v>
@@ -2022,7 +2032,7 @@
         <v>27</v>
       </c>
       <c r="O30" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="P30" s="1" t="s">
         <v>28</v>
@@ -2060,7 +2070,7 @@
         <v>echo $p116."=p116&lt;br&gt;";</v>
       </c>
       <c r="L31" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="M31" t="s">
         <v>26</v>
@@ -2069,7 +2079,7 @@
         <v>27</v>
       </c>
       <c r="O31" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="P31" s="1" t="s">
         <v>28</v>
@@ -2107,7 +2117,7 @@
         <v>echo $p117."=p117&lt;br&gt;";</v>
       </c>
       <c r="L32" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="M32" t="s">
         <v>26</v>
@@ -2116,7 +2126,7 @@
         <v>27</v>
       </c>
       <c r="O32" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="P32" s="1" t="s">
         <v>28</v>
@@ -2154,7 +2164,7 @@
         <v>echo $p118."=p118&lt;br&gt;";</v>
       </c>
       <c r="L33" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="M33" t="s">
         <v>26</v>
@@ -2163,7 +2173,7 @@
         <v>27</v>
       </c>
       <c r="O33" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="P33" s="1" t="s">
         <v>28</v>
@@ -2188,7 +2198,7 @@
         <v>echo $p119."=p119&lt;br&gt;";</v>
       </c>
       <c r="L34" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="M34" t="s">
         <v>26</v>
@@ -2197,7 +2207,7 @@
         <v>27</v>
       </c>
       <c r="O34" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="P34" s="1" t="s">
         <v>28</v>
@@ -2222,7 +2232,7 @@
         <v>echo $p120."=p120&lt;br&gt;";</v>
       </c>
       <c r="L35" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="M35" t="s">
         <v>26</v>
@@ -2231,7 +2241,7 @@
         <v>27</v>
       </c>
       <c r="O35" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="P35" s="1" t="s">
         <v>28</v>
@@ -2256,7 +2266,7 @@
         <v>echo $p121."=p121&lt;br&gt;";</v>
       </c>
       <c r="L36" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="M36" t="s">
         <v>26</v>
@@ -2265,7 +2275,7 @@
         <v>27</v>
       </c>
       <c r="O36" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="P36" s="1" t="s">
         <v>28</v>
@@ -2290,7 +2300,7 @@
         <v>echo $p122."=p122&lt;br&gt;";</v>
       </c>
       <c r="L37" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="M37" t="s">
         <v>26</v>
@@ -2299,7 +2309,7 @@
         <v>27</v>
       </c>
       <c r="O37" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="P37" s="1" t="s">
         <v>28</v>
@@ -2313,4 +2323,313 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FDA0078-5A29-437F-8476-FC551A3367CB}">
+  <dimension ref="B1:H14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:H14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H1" t="str">
+        <f>CONCATENATE(B1,C1,D1,E1,F1)</f>
+        <v>$p1_52 = $_POST['p1_52'];</v>
+      </c>
+    </row>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H2" t="str">
+        <f t="shared" ref="H2:H14" si="0">CONCATENATE(B2,C2,D2,E2,F2)</f>
+        <v>$p1_53 = $_POST['p1_53'];</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H3" t="str">
+        <f t="shared" si="0"/>
+        <v>$p1_54 = $_POST['p1_54'];</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E4" t="s">
+        <v>67</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H4" t="str">
+        <f t="shared" si="0"/>
+        <v>$p1_55 = $_POST['p1_55'];</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D5" t="s">
+        <v>79</v>
+      </c>
+      <c r="E5" t="s">
+        <v>68</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H5" t="str">
+        <f t="shared" si="0"/>
+        <v>$p1_56 = $_POST['p1_56'];</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E6" t="s">
+        <v>69</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" si="0"/>
+        <v>$p1_57 = $_POST['p1_57'];</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7" t="s">
+        <v>70</v>
+      </c>
+      <c r="D7" t="s">
+        <v>79</v>
+      </c>
+      <c r="E7" t="s">
+        <v>70</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" si="0"/>
+        <v>$p1_58 = $_POST['p1_58'];</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" t="s">
+        <v>71</v>
+      </c>
+      <c r="D8" t="s">
+        <v>79</v>
+      </c>
+      <c r="E8" t="s">
+        <v>71</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H8" t="str">
+        <f t="shared" si="0"/>
+        <v>$p1_59 = $_POST['p1_59'];</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9" t="s">
+        <v>72</v>
+      </c>
+      <c r="D9" t="s">
+        <v>79</v>
+      </c>
+      <c r="E9" t="s">
+        <v>72</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H9" t="str">
+        <f t="shared" si="0"/>
+        <v>$p1_60 = $_POST['p1_60'];</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10" t="s">
+        <v>73</v>
+      </c>
+      <c r="D10" t="s">
+        <v>79</v>
+      </c>
+      <c r="E10" t="s">
+        <v>73</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H10" t="str">
+        <f t="shared" si="0"/>
+        <v>$p1_61 = $_POST['p1_61'];</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>78</v>
+      </c>
+      <c r="C11" t="s">
+        <v>74</v>
+      </c>
+      <c r="D11" t="s">
+        <v>79</v>
+      </c>
+      <c r="E11" t="s">
+        <v>74</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H11" t="str">
+        <f t="shared" si="0"/>
+        <v>$p1_62 = $_POST['p1_62'];</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C12" t="s">
+        <v>75</v>
+      </c>
+      <c r="D12" t="s">
+        <v>79</v>
+      </c>
+      <c r="E12" t="s">
+        <v>75</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H12" t="str">
+        <f t="shared" si="0"/>
+        <v>$p1_63 = $_POST['p1_63'];</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>78</v>
+      </c>
+      <c r="C13" t="s">
+        <v>76</v>
+      </c>
+      <c r="D13" t="s">
+        <v>79</v>
+      </c>
+      <c r="E13" t="s">
+        <v>76</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H13" t="str">
+        <f t="shared" si="0"/>
+        <v>$p1_64 = $_POST['p1_64'];</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C14" t="s">
+        <v>77</v>
+      </c>
+      <c r="D14" t="s">
+        <v>79</v>
+      </c>
+      <c r="E14" t="s">
+        <v>77</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H14" t="str">
+        <f t="shared" si="0"/>
+        <v>$p1_65 = $_POST['p1_65'];</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>